<commit_message>
fix tmpl path import
</commit_message>
<xml_diff>
--- a/exmple/accounts.xlsx
+++ b/exmple/accounts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="permissions" sheetId="1" state="visible" r:id="rId3"/>
@@ -13,6 +13,7 @@
     <sheet name="translations" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="navigation bars" sheetId="4" state="visible" r:id="rId6"/>
     <sheet name="buckets" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="users" sheetId="6" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'navigation bars'!$A$1:$G$12</definedName>
@@ -27,18 +28,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="241">
-  <si>
-    <t xml:space="preserve">permission name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">permission function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">permission group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">permission description</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="255">
+  <si>
+    <t xml:space="preserve">permission_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">permission_function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">permission_group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">permission_description</t>
   </si>
   <si>
     <t xml:space="preserve">roles list</t>
@@ -284,7 +285,7 @@
     <t xml:space="preserve">role_name</t>
   </si>
   <si>
-    <t xml:space="preserve">role_group#</t>
+    <t xml:space="preserve">role_group</t>
   </si>
   <si>
     <t xml:space="preserve">permission_id***accounts_schema.role_permissions***accounts_schema.permissions***permission_functions***role_name</t>
@@ -299,457 +300,499 @@
     <t xml:space="preserve">*</t>
   </si>
   <si>
-    <t xml:space="preserve">super admin2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">super admin role2</t>
+    <t xml:space="preserve">modirtator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NavigationList|NavigationCreate|NavigationUpdate|NavigationDelete|NavigationRestore|IconsList|IconCreateIconUpdate|IconDelete|IconRestore|TranslationsList|TranslationCreate|TranslationUpdate|TranslationDelete|TranslationRestore  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">translation_key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">english value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arabic value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roles.list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List Roles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شوف الأدوار</t>
+  </si>
+  <si>
+    <t xml:space="preserve">role.create</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">اعمل دور</t>
+  </si>
+  <si>
+    <t xml:space="preserve">role.update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update Role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">عدل الدور</t>
+  </si>
+  <si>
+    <t xml:space="preserve">role.delete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete Role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">احذف الدور</t>
+  </si>
+  <si>
+    <t xml:space="preserve">role.restore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restore Role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">رجع الدور</t>
+  </si>
+  <si>
+    <t xml:space="preserve">users.list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List Users</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شوف المستخدمين</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user.create</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">اعمل مستخدم</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user.update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">عدل المستخدم</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user.delete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">احذف المستخدم</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user.restore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restore User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">رجع المستخدم</t>
+  </si>
+  <si>
+    <t xml:space="preserve">navigation.list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List Navigation Items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شوف عناصر التنقل</t>
+  </si>
+  <si>
+    <t xml:space="preserve">navigation.create</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Navigation Item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">اعمل عنصر تنقل</t>
+  </si>
+  <si>
+    <t xml:space="preserve">navigation.update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update Navigation Item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">عدل عنصر التنقل</t>
+  </si>
+  <si>
+    <t xml:space="preserve">navigation.delete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete Navigation Item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">احذف عنصر التنقل</t>
+  </si>
+  <si>
+    <t xml:space="preserve">navigation.restore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restore Navigation Item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">رجع عنصر التنقل</t>
+  </si>
+  <si>
+    <t xml:space="preserve">icons.list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List Icons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شوف الأيقونات</t>
+  </si>
+  <si>
+    <t xml:space="preserve">icon.create</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">اعمل أيقونة</t>
+  </si>
+  <si>
+    <t xml:space="preserve">icon.update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update Icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">عدل الأيقونة</t>
+  </si>
+  <si>
+    <t xml:space="preserve">icon.delete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete Icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">احذف الأيقونة</t>
+  </si>
+  <si>
+    <t xml:space="preserve">icon.restore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restore Icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">رجع الأيقونة</t>
+  </si>
+  <si>
+    <t xml:space="preserve">translations.list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List Translations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شوف الترجمات</t>
+  </si>
+  <si>
+    <t xml:space="preserve">translation.create</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Translation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">اعمل ترجمة</t>
+  </si>
+  <si>
+    <t xml:space="preserve">translation.update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update Translation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">عدل الترجمة</t>
+  </si>
+  <si>
+    <t xml:space="preserve">translation.delete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete Translation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">احذف الترجمة</t>
+  </si>
+  <si>
+    <t xml:space="preserve">translation.restore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restore Translation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">رجع الترجمة</t>
+  </si>
+  <si>
+    <t xml:space="preserve">menu_key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label_ar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">route</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parent_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">permission_id**accounts_schema.permissions**permission_function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dashboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dashboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">لوحة التحكم</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dashboard_icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/dashboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DashboardView</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accounts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accounts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">الحسابات</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accounts_icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/accounts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AccountsView</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">الأدوار</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roles_icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/accounts/roles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Users</t>
+  </si>
+  <si>
+    <t xml:space="preserve">المستخدمين</t>
+  </si>
+  <si>
+    <t xml:space="preserve">users_icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/accounts/users</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navigation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">التنقل</t>
+  </si>
+  <si>
+    <t xml:space="preserve">navigation_icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/accounts/navigation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">النظام</t>
+  </si>
+  <si>
+    <t xml:space="preserve">system_icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SystemView</t>
+  </si>
+  <si>
+    <t xml:space="preserve">settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">الإعدادات</t>
+  </si>
+  <si>
+    <t xml:space="preserve">settings_icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/system/settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SettingsView</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Translations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">الترجمات</t>
+  </si>
+  <si>
+    <t xml:space="preserve">translations_icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/system/translations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Icons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">الأيقونات</t>
+  </si>
+  <si>
+    <t xml:space="preserve">icons_icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/system/icons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buckets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buckets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">الدلاء</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buckets_icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/system/buckets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BucketsList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">objects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">الكائنات</t>
+  </si>
+  <si>
+    <t xml:space="preserve">objects_icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/system/objects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ObjectsList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bucket name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is public</t>
+  </si>
+  <si>
+    <t xml:space="preserve">images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_security_level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_type_id**accounts_schema.user_types**user_type_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_password#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">role_id***accounts_schema.user_roles***accounts_schema.roles***role_name***user_email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ahmed</t>
   </si>
   <si>
     <t xml:space="preserve">admin</t>
   </si>
   <si>
-    <t xml:space="preserve">super admin3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">super admin role3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">list|update</t>
-  </si>
-  <si>
-    <t xml:space="preserve">translation_key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">english value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">arabic value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">roles.list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List Roles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">شوف الأدوار</t>
-  </si>
-  <si>
-    <t xml:space="preserve">role.create</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create Role</t>
-  </si>
-  <si>
-    <t xml:space="preserve">اعمل دور</t>
-  </si>
-  <si>
-    <t xml:space="preserve">role.update</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update Role</t>
-  </si>
-  <si>
-    <t xml:space="preserve">عدل الدور</t>
-  </si>
-  <si>
-    <t xml:space="preserve">role.delete</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete Role</t>
-  </si>
-  <si>
-    <t xml:space="preserve">احذف الدور</t>
-  </si>
-  <si>
-    <t xml:space="preserve">role.restore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Restore Role</t>
-  </si>
-  <si>
-    <t xml:space="preserve">رجع الدور</t>
-  </si>
-  <si>
-    <t xml:space="preserve">users.list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List Users</t>
-  </si>
-  <si>
-    <t xml:space="preserve">شوف المستخدمين</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user.create</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create User</t>
-  </si>
-  <si>
-    <t xml:space="preserve">اعمل مستخدم</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user.update</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update User</t>
-  </si>
-  <si>
-    <t xml:space="preserve">عدل المستخدم</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user.delete</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete User</t>
-  </si>
-  <si>
-    <t xml:space="preserve">احذف المستخدم</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user.restore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Restore User</t>
-  </si>
-  <si>
-    <t xml:space="preserve">رجع المستخدم</t>
-  </si>
-  <si>
-    <t xml:space="preserve">navigation.list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List Navigation Items</t>
-  </si>
-  <si>
-    <t xml:space="preserve">شوف عناصر التنقل</t>
-  </si>
-  <si>
-    <t xml:space="preserve">navigation.create</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create Navigation Item</t>
-  </si>
-  <si>
-    <t xml:space="preserve">اعمل عنصر تنقل</t>
-  </si>
-  <si>
-    <t xml:space="preserve">navigation.update</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update Navigation Item</t>
-  </si>
-  <si>
-    <t xml:space="preserve">عدل عنصر التنقل</t>
-  </si>
-  <si>
-    <t xml:space="preserve">navigation.delete</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete Navigation Item</t>
-  </si>
-  <si>
-    <t xml:space="preserve">احذف عنصر التنقل</t>
-  </si>
-  <si>
-    <t xml:space="preserve">navigation.restore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Restore Navigation Item</t>
-  </si>
-  <si>
-    <t xml:space="preserve">رجع عنصر التنقل</t>
-  </si>
-  <si>
-    <t xml:space="preserve">icons.list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List Icons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">شوف الأيقونات</t>
-  </si>
-  <si>
-    <t xml:space="preserve">icon.create</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create Icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">اعمل أيقونة</t>
-  </si>
-  <si>
-    <t xml:space="preserve">icon.update</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update Icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">عدل الأيقونة</t>
-  </si>
-  <si>
-    <t xml:space="preserve">icon.delete</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete Icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">احذف الأيقونة</t>
-  </si>
-  <si>
-    <t xml:space="preserve">icon.restore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Restore Icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">رجع الأيقونة</t>
-  </si>
-  <si>
-    <t xml:space="preserve">translations.list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List Translations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">شوف الترجمات</t>
-  </si>
-  <si>
-    <t xml:space="preserve">translation.create</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create Translation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">اعمل ترجمة</t>
-  </si>
-  <si>
-    <t xml:space="preserve">translation.update</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update Translation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">عدل الترجمة</t>
-  </si>
-  <si>
-    <t xml:space="preserve">translation.delete</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete Translation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">احذف الترجمة</t>
-  </si>
-  <si>
-    <t xml:space="preserve">translation.restore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Restore Translation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">رجع الترجمة</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Menu Key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Label (Arabic)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Route</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parent ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Permission Function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dashboard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dashboard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">لوحة التحكم</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dashboard_icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/dashboard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DashboardView</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accounts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accounts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">الحسابات</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accounts_icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/accounts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AccountsView</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">الأدوار</t>
-  </si>
-  <si>
-    <t xml:space="preserve">roles_icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/accounts/roles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Users</t>
-  </si>
-  <si>
-    <t xml:space="preserve">المستخدمين</t>
-  </si>
-  <si>
-    <t xml:space="preserve">users_icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/accounts/users</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Navigation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">التنقل</t>
-  </si>
-  <si>
-    <t xml:space="preserve">navigation_icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/accounts/navigation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">System</t>
-  </si>
-  <si>
-    <t xml:space="preserve">النظام</t>
-  </si>
-  <si>
-    <t xml:space="preserve">system_icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SystemView</t>
-  </si>
-  <si>
-    <t xml:space="preserve">settings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Settings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">الإعدادات</t>
-  </si>
-  <si>
-    <t xml:space="preserve">settings_icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/system/settings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SettingsView</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Translations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">الترجمات</t>
-  </si>
-  <si>
-    <t xml:space="preserve">translations_icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/system/translations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Icons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">الأيقونات</t>
-  </si>
-  <si>
-    <t xml:space="preserve">icons_icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/system/icons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">buckets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buckets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">الدلاء</t>
-  </si>
-  <si>
-    <t xml:space="preserve">buckets_icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/system/buckets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BucketsList</t>
-  </si>
-  <si>
-    <t xml:space="preserve">objects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Objects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">الكائنات</t>
-  </si>
-  <si>
-    <t xml:space="preserve">objects_icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/system/objects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ObjectsList</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bucket name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is public</t>
-  </si>
-  <si>
-    <t xml:space="preserve">images</t>
+    <t xml:space="preserve">ahmed@devkit.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yossuf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yossuf@devkit.cmoyossuf@mln.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modirator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">karim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 1118614244</t>
+  </si>
+  <si>
+    <t xml:space="preserve">karim@devkit.com</t>
   </si>
 </sst>
 </file>
@@ -760,7 +803,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -795,6 +838,12 @@
       <name val="CommitMono Nerd Font"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -845,7 +894,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -871,6 +920,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -919,20 +980,20 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:D28" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A1:D28"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="permission name"/>
-    <tableColumn id="2" name="permission function"/>
-    <tableColumn id="3" name="permission group"/>
-    <tableColumn id="4" name="permission description"/>
+    <tableColumn id="1" name="permission_name"/>
+    <tableColumn id="2" name="permission_function"/>
+    <tableColumn id="3" name="permission_group"/>
+    <tableColumn id="4" name="permission_description"/>
   </tableColumns>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table3" displayName="Table3" ref="A1:C4" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:C4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table3" displayName="Table3" ref="A1:C3" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:C3"/>
   <tableColumns count="3">
     <tableColumn id="1" name="role_name"/>
-    <tableColumn id="2" name="role_group#"/>
+    <tableColumn id="2" name="role_group"/>
     <tableColumn id="3" name="permission_id***accounts_schema.role_permissions***accounts_schema.permissions***permission_functions***role_name"/>
   </tableColumns>
 </table>
@@ -1129,7 +1190,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1523,17 +1584,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J28" activeCellId="0" sqref="J28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="94.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="42.01"/>
   </cols>
   <sheetData>
@@ -1571,29 +1632,47 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="3"/>
+    </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1602,7 +1681,7 @@
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.700694444444445" right="0.700694444444445" top="0.752083333333333" bottom="0.752083333333333" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1638,288 +1717,288 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1944,85 +2023,86 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G32" activeCellId="0" sqref="G32"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="12.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="20.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="57.48"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>177</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="F2" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>184</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="F3" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>190</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2030,16 +2110,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>197</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>2</v>
@@ -2053,16 +2133,16 @@
         <v>22</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>198</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>201</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>2</v>
@@ -2076,16 +2156,16 @@
         <v>38</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>202</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>205</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>2</v>
@@ -2096,48 +2176,48 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="F7" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>208</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>213</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>216</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>7</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2145,16 +2225,16 @@
         <v>70</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>218</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>221</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>7</v>
@@ -2168,16 +2248,16 @@
         <v>54</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>225</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>7</v>
@@ -2188,48 +2268,48 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>227</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>230</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>7</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>233</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>236</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>7</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -2253,22 +2333,26 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.93"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B2" s="6" t="n">
         <f aca="false">TRUE()</f>
@@ -2294,4 +2378,133 @@
     <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G31"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C58" activeCellId="0" sqref="C58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="58.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="34.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.41"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="D2" s="7" t="n">
+        <v>1022052546</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="F2" s="8" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="D3" s="7" t="n">
+        <v>1202290100</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="F3" s="8" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="F4" s="8" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="ahmed@devkit.com"/>
+    <hyperlink ref="E4" r:id="rId2" display="karim@devkit.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>